<commit_message>
Atualizando o Burndown da segunda sprint e renomeando os documentos de casos de testes
</commit_message>
<xml_diff>
--- a/docs/sprint2/burndown_sprint2.xlsx
+++ b/docs/sprint2/burndown_sprint2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55129\Documents\Fatec\2 Semestre\API\documentacao\sprint2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\55129\Documents\Fatec\2 Semestre\API\repositorio\docs\sprint2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B71F99B-4116-4D84-9C20-282A50D502F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A163EBC-673D-46D1-9956-C3015FF47D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4188" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -409,28 +409,37 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -441,15 +450,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -605,67 +605,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>114</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108.3</c:v>
+                  <c:v>109.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>102.6</c:v>
+                  <c:v>103.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>96.899999999999991</c:v>
+                  <c:v>97.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91.199999999999989</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>85.499999999999986</c:v>
+                  <c:v>86.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>79.799999999999983</c:v>
+                  <c:v>80.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>74.09999999999998</c:v>
+                  <c:v>74.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>68.399999999999977</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>62.699999999999974</c:v>
+                  <c:v>63.25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>56.999999999999972</c:v>
+                  <c:v>57.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>51.299999999999969</c:v>
+                  <c:v>51.75</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45.599999999999966</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>39.899999999999963</c:v>
+                  <c:v>40.25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>34.19999999999996</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28.499999999999961</c:v>
+                  <c:v>28.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22.799999999999962</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.099999999999962</c:v>
+                  <c:v>17.25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.399999999999963</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.6999999999999629</c:v>
+                  <c:v>5.75</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-3.730349362740526E-14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -770,61 +770,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>114</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>114</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>114</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>114</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>114</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>114</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>98</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>98</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>91</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>79</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>64</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>60</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>58</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>39</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>35</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>32</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -1272,8 +1272,8 @@
   </sheetPr>
   <dimension ref="A1:N1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="E61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K72" sqref="K72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="C5" s="6">
         <f>SUM(J29:J1006)</f>
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" ref="D5:D25" si="0">SUMIF($K$29:$K$1006,B5,$J$29:$J$1006)</f>
@@ -1345,7 +1345,7 @@
       </c>
       <c r="E5" s="6">
         <f>C5-D5</f>
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
@@ -1358,7 +1358,7 @@
       </c>
       <c r="C6" s="6">
         <f t="shared" ref="C6:C25" si="2">C5-$C$5/($B$2-1)</f>
-        <v>108.3</v>
+        <v>109.25</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" si="0"/>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="E6" s="6">
         <f t="shared" ref="E6:E25" ca="1" si="3">IF(B6&lt;=$E$1,E5-D6,)</f>
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="C7" s="6">
         <f t="shared" si="2"/>
-        <v>102.6</v>
+        <v>103.5</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="0"/>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="E7" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
@@ -1400,7 +1400,7 @@
       </c>
       <c r="C8" s="6">
         <f t="shared" si="2"/>
-        <v>96.899999999999991</v>
+        <v>97.75</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="E8" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="C9" s="6">
         <f t="shared" si="2"/>
-        <v>91.199999999999989</v>
+        <v>92</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="0"/>
@@ -1429,7 +1429,7 @@
       </c>
       <c r="E9" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="C10" s="6">
         <f t="shared" si="2"/>
-        <v>85.499999999999986</v>
+        <v>86.25</v>
       </c>
       <c r="D10" s="6">
         <f t="shared" si="0"/>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="E10" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="C11" s="6">
         <f t="shared" si="2"/>
-        <v>79.799999999999983</v>
+        <v>80.5</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" si="0"/>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="E11" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
@@ -1484,7 +1484,7 @@
       </c>
       <c r="C12" s="6">
         <f t="shared" si="2"/>
-        <v>74.09999999999998</v>
+        <v>74.75</v>
       </c>
       <c r="D12" s="6">
         <f t="shared" si="0"/>
@@ -1492,7 +1492,7 @@
       </c>
       <c r="E12" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
@@ -1505,7 +1505,7 @@
       </c>
       <c r="C13" s="6">
         <f t="shared" si="2"/>
-        <v>68.399999999999977</v>
+        <v>69</v>
       </c>
       <c r="D13" s="6">
         <f t="shared" si="0"/>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="E13" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="C14" s="6">
         <f t="shared" si="2"/>
-        <v>62.699999999999974</v>
+        <v>63.25</v>
       </c>
       <c r="D14" s="6">
         <f t="shared" si="0"/>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="E14" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
@@ -1547,7 +1547,7 @@
       </c>
       <c r="C15" s="6">
         <f t="shared" si="2"/>
-        <v>56.999999999999972</v>
+        <v>57.5</v>
       </c>
       <c r="D15" s="6">
         <f t="shared" si="0"/>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="E15" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="C16" s="6">
         <f t="shared" si="2"/>
-        <v>51.299999999999969</v>
+        <v>51.75</v>
       </c>
       <c r="D16" s="6">
         <f t="shared" si="0"/>
@@ -1576,7 +1576,7 @@
       </c>
       <c r="E16" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
@@ -1589,7 +1589,7 @@
       </c>
       <c r="C17" s="6">
         <f t="shared" si="2"/>
-        <v>45.599999999999966</v>
+        <v>46</v>
       </c>
       <c r="D17" s="6">
         <f t="shared" si="0"/>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="E17" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
@@ -1610,7 +1610,7 @@
       </c>
       <c r="C18" s="6">
         <f t="shared" si="2"/>
-        <v>39.899999999999963</v>
+        <v>40.25</v>
       </c>
       <c r="D18" s="6">
         <f t="shared" si="0"/>
@@ -1618,7 +1618,7 @@
       </c>
       <c r="E18" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="C19" s="6">
         <f t="shared" si="2"/>
-        <v>34.19999999999996</v>
+        <v>34.5</v>
       </c>
       <c r="D19" s="6">
         <f t="shared" si="0"/>
@@ -1639,7 +1639,7 @@
       </c>
       <c r="E19" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
@@ -1652,7 +1652,7 @@
       </c>
       <c r="C20" s="6">
         <f t="shared" si="2"/>
-        <v>28.499999999999961</v>
+        <v>28.75</v>
       </c>
       <c r="D20" s="6">
         <f t="shared" si="0"/>
@@ -1660,7 +1660,7 @@
       </c>
       <c r="E20" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="C21" s="6">
         <f t="shared" si="2"/>
-        <v>22.799999999999962</v>
+        <v>23</v>
       </c>
       <c r="D21" s="6">
         <f t="shared" si="0"/>
@@ -1681,7 +1681,7 @@
       </c>
       <c r="E21" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F21" s="14"/>
     </row>
@@ -1695,7 +1695,7 @@
       </c>
       <c r="C22" s="6">
         <f t="shared" si="2"/>
-        <v>17.099999999999962</v>
+        <v>17.25</v>
       </c>
       <c r="D22" s="6">
         <f t="shared" si="0"/>
@@ -1703,7 +1703,7 @@
       </c>
       <c r="E22" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
@@ -1716,7 +1716,7 @@
       </c>
       <c r="C23" s="6">
         <f t="shared" si="2"/>
-        <v>11.399999999999963</v>
+        <v>11.5</v>
       </c>
       <c r="D23" s="6">
         <f t="shared" si="0"/>
@@ -1724,7 +1724,7 @@
       </c>
       <c r="E23" s="6">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
@@ -1737,11 +1737,11 @@
       </c>
       <c r="C24" s="6">
         <f t="shared" si="2"/>
-        <v>5.6999999999999629</v>
+        <v>5.75</v>
       </c>
       <c r="D24" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="6">
         <f t="shared" ca="1" si="3"/>
@@ -1758,7 +1758,7 @@
       </c>
       <c r="C25" s="6">
         <f t="shared" si="2"/>
-        <v>-3.730349362740526E-14</v>
+        <v>0</v>
       </c>
       <c r="D25" s="6">
         <f t="shared" si="0"/>
@@ -1773,54 +1773,54 @@
       <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="30"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
     </row>
     <row r="28" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="33" t="s">
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="I28" s="34" t="s">
+      <c r="I28" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="J28" s="34" t="s">
+      <c r="J28" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="K28" s="34" t="s">
+      <c r="K28" s="22" t="s">
         <v>13</v>
       </c>
       <c r="L28" s="3"/>
     </row>
     <row r="29" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
       <c r="H29" s="15">
         <v>45029</v>
       </c>
@@ -1837,15 +1837,15 @@
       <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
       <c r="H30" s="15">
         <v>45028</v>
       </c>
@@ -1862,15 +1862,15 @@
       <c r="N30" s="3"/>
     </row>
     <row r="31" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
       <c r="H31" s="18">
         <v>45029</v>
       </c>
@@ -1886,15 +1886,15 @@
       <c r="L31" s="4"/>
     </row>
     <row r="32" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
       <c r="H32" s="15">
         <v>45028</v>
       </c>
@@ -1910,15 +1910,15 @@
       <c r="L32" s="4"/>
     </row>
     <row r="33" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
       <c r="H33" s="15">
         <v>45025</v>
       </c>
@@ -1934,15 +1934,15 @@
       <c r="L33" s="4"/>
     </row>
     <row r="34" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
       <c r="H34" s="15">
         <v>45027</v>
       </c>
@@ -1958,15 +1958,15 @@
       <c r="L34" s="4"/>
     </row>
     <row r="35" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
       <c r="H35" s="18">
         <v>45022</v>
       </c>
@@ -1982,15 +1982,15 @@
       <c r="L35" s="4"/>
     </row>
     <row r="36" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="28"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
       <c r="H36" s="18">
         <v>45022</v>
       </c>
@@ -2006,15 +2006,15 @@
       <c r="L36" s="4"/>
     </row>
     <row r="37" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
       <c r="H37" s="18">
         <v>45025</v>
       </c>
@@ -2030,15 +2030,15 @@
       <c r="L37" s="4"/>
     </row>
     <row r="38" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
       <c r="H38" s="18">
         <v>45025</v>
       </c>
@@ -2054,15 +2054,15 @@
       <c r="L38" s="4"/>
     </row>
     <row r="39" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
       <c r="H39" s="18">
         <v>45025</v>
       </c>
@@ -2078,15 +2078,15 @@
       <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="28"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
       <c r="H40" s="18">
         <v>45029</v>
       </c>
@@ -2102,15 +2102,15 @@
       <c r="L40" s="4"/>
     </row>
     <row r="41" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
       <c r="H41" s="18">
         <v>45029</v>
       </c>
@@ -2126,15 +2126,15 @@
       <c r="L41" s="4"/>
     </row>
     <row r="42" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
       <c r="H42" s="18">
         <v>45027</v>
       </c>
@@ -2150,15 +2150,15 @@
       <c r="L42" s="4"/>
     </row>
     <row r="43" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
       <c r="H43" s="18">
         <v>45025</v>
       </c>
@@ -2174,15 +2174,15 @@
       <c r="L43" s="4"/>
     </row>
     <row r="44" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
       <c r="H44" s="18">
         <v>45028</v>
       </c>
@@ -2198,15 +2198,15 @@
       <c r="L44" s="4"/>
     </row>
     <row r="45" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
       <c r="H45" s="18">
         <v>45031</v>
       </c>
@@ -2222,15 +2222,15 @@
       <c r="L45" s="4"/>
     </row>
     <row r="46" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="25" t="s">
+      <c r="A46" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="28"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
       <c r="H46" s="18">
         <v>45031</v>
       </c>
@@ -2246,15 +2246,15 @@
       <c r="L46" s="4"/>
     </row>
     <row r="47" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B47" s="28"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="28"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
       <c r="H47" s="18">
         <v>45028</v>
       </c>
@@ -2270,15 +2270,15 @@
       <c r="L47" s="4"/>
     </row>
     <row r="48" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="B48" s="28"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="28"/>
-      <c r="F48" s="28"/>
-      <c r="G48" s="28"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="25"/>
       <c r="H48" s="18">
         <v>45031</v>
       </c>
@@ -2294,15 +2294,15 @@
       <c r="L48" s="4"/>
     </row>
     <row r="49" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="28"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
       <c r="H49" s="18">
         <v>45030</v>
       </c>
@@ -2318,15 +2318,15 @@
       <c r="L49" s="4"/>
     </row>
     <row r="50" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A50" s="35" t="s">
+      <c r="A50" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="28"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
       <c r="H50" s="18">
         <v>45034</v>
       </c>
@@ -2342,15 +2342,15 @@
       <c r="L50" s="4"/>
     </row>
     <row r="51" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A51" s="25" t="s">
+      <c r="A51" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="28"/>
-      <c r="F51" s="28"/>
-      <c r="G51" s="28"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
       <c r="H51" s="18">
         <v>45028</v>
       </c>
@@ -2366,15 +2366,15 @@
       <c r="L51" s="4"/>
     </row>
     <row r="52" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
+      <c r="A52" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="28"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="25"/>
       <c r="H52" s="18">
         <v>45028</v>
       </c>
@@ -2390,15 +2390,15 @@
       <c r="L52" s="4"/>
     </row>
     <row r="53" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A53" s="25" t="s">
+      <c r="A53" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="28"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
       <c r="H53" s="18">
         <v>45030</v>
       </c>
@@ -2414,15 +2414,15 @@
       <c r="L53" s="4"/>
     </row>
     <row r="54" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="28"/>
-      <c r="G54" s="28"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
       <c r="H54" s="18">
         <v>45029</v>
       </c>
@@ -2438,15 +2438,15 @@
       <c r="L54" s="4"/>
     </row>
     <row r="55" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="25" t="s">
+      <c r="A55" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B55" s="28"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="28"/>
-      <c r="G55" s="28"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
       <c r="H55" s="18">
         <v>45031</v>
       </c>
@@ -2462,15 +2462,15 @@
       <c r="L55" s="4"/>
     </row>
     <row r="56" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="28"/>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="28"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="25"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="25"/>
       <c r="H56" s="18">
         <v>45031</v>
       </c>
@@ -2486,15 +2486,15 @@
       <c r="L56" s="4"/>
     </row>
     <row r="57" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A57" s="25" t="s">
+      <c r="A57" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B57" s="28"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="28"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="25"/>
+      <c r="G57" s="25"/>
       <c r="H57" s="18">
         <v>45031</v>
       </c>
@@ -2510,15 +2510,15 @@
       <c r="L57" s="4"/>
     </row>
     <row r="58" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A58" s="25" t="s">
+      <c r="A58" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B58" s="28"/>
-      <c r="C58" s="28"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="28"/>
-      <c r="F58" s="28"/>
-      <c r="G58" s="28"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
       <c r="H58" s="18">
         <v>45032</v>
       </c>
@@ -2534,15 +2534,15 @@
       <c r="L58" s="4"/>
     </row>
     <row r="59" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A59" s="25" t="s">
+      <c r="A59" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B59" s="28"/>
-      <c r="C59" s="28"/>
-      <c r="D59" s="28"/>
-      <c r="E59" s="28"/>
-      <c r="F59" s="28"/>
-      <c r="G59" s="28"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="25"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="25"/>
+      <c r="F59" s="25"/>
+      <c r="G59" s="25"/>
       <c r="H59" s="18">
         <v>45033</v>
       </c>
@@ -2558,15 +2558,15 @@
       <c r="L59" s="4"/>
     </row>
     <row r="60" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A60" s="28" t="s">
+      <c r="A60" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B60" s="28"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="28"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="25"/>
       <c r="H60" s="18">
         <v>45037</v>
       </c>
@@ -2582,15 +2582,15 @@
       <c r="L60" s="4"/>
     </row>
     <row r="61" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A61" s="28" t="s">
+      <c r="A61" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="28"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="28"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="28"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="25"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="25"/>
+      <c r="G61" s="25"/>
       <c r="H61" s="18">
         <v>45032</v>
       </c>
@@ -2606,15 +2606,15 @@
       <c r="L61" s="4"/>
     </row>
     <row r="62" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A62" s="28" t="s">
+      <c r="A62" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B62" s="28"/>
-      <c r="C62" s="28"/>
-      <c r="D62" s="28"/>
-      <c r="E62" s="28"/>
-      <c r="F62" s="28"/>
-      <c r="G62" s="28"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="25"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="25"/>
       <c r="H62" s="18">
         <v>45031</v>
       </c>
@@ -2630,15 +2630,15 @@
       <c r="L62" s="4"/>
     </row>
     <row r="63" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A63" s="28" t="s">
+      <c r="A63" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B63" s="28"/>
-      <c r="C63" s="28"/>
-      <c r="D63" s="28"/>
-      <c r="E63" s="28"/>
-      <c r="F63" s="28"/>
-      <c r="G63" s="28"/>
+      <c r="B63" s="25"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="25"/>
+      <c r="F63" s="25"/>
+      <c r="G63" s="25"/>
       <c r="H63" s="18">
         <v>45034</v>
       </c>
@@ -2654,15 +2654,15 @@
       <c r="L63" s="4"/>
     </row>
     <row r="64" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A64" s="25" t="s">
+      <c r="A64" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B64" s="28"/>
-      <c r="C64" s="28"/>
-      <c r="D64" s="28"/>
-      <c r="E64" s="28"/>
-      <c r="F64" s="28"/>
-      <c r="G64" s="28"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="25"/>
+      <c r="G64" s="25"/>
       <c r="H64" s="18">
         <v>45034</v>
       </c>
@@ -2678,15 +2678,15 @@
       <c r="L64" s="4"/>
     </row>
     <row r="65" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A65" s="29" t="s">
+      <c r="A65" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B65" s="22"/>
-      <c r="C65" s="22"/>
-      <c r="D65" s="22"/>
-      <c r="E65" s="22"/>
-      <c r="F65" s="22"/>
-      <c r="G65" s="23"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="27"/>
+      <c r="E65" s="27"/>
+      <c r="F65" s="27"/>
+      <c r="G65" s="28"/>
       <c r="H65" s="18">
         <v>45034</v>
       </c>
@@ -2702,15 +2702,15 @@
       <c r="L65" s="4"/>
     </row>
     <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="25" t="s">
+      <c r="A66" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="B66" s="28"/>
-      <c r="C66" s="28"/>
-      <c r="D66" s="28"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="28"/>
-      <c r="G66" s="28"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="25"/>
+      <c r="G66" s="25"/>
       <c r="H66" s="18">
         <v>45034</v>
       </c>
@@ -2729,12 +2729,12 @@
       <c r="A67" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="B67" s="22"/>
-      <c r="C67" s="22"/>
-      <c r="D67" s="22"/>
-      <c r="E67" s="22"/>
-      <c r="F67" s="22"/>
-      <c r="G67" s="23"/>
+      <c r="B67" s="27"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="27"/>
+      <c r="E67" s="27"/>
+      <c r="F67" s="27"/>
+      <c r="G67" s="28"/>
       <c r="H67" s="18">
         <v>45036</v>
       </c>
@@ -2753,12 +2753,12 @@
       <c r="A68" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="22"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="22"/>
-      <c r="E68" s="22"/>
-      <c r="F68" s="22"/>
-      <c r="G68" s="23"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="27"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="28"/>
       <c r="H68" s="18">
         <v>45036</v>
       </c>
@@ -2777,12 +2777,12 @@
       <c r="A69" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="B69" s="22"/>
-      <c r="C69" s="22"/>
-      <c r="D69" s="22"/>
-      <c r="E69" s="22"/>
-      <c r="F69" s="22"/>
-      <c r="G69" s="23"/>
+      <c r="B69" s="27"/>
+      <c r="C69" s="27"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="27"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="28"/>
       <c r="H69" s="18">
         <v>45036</v>
       </c>
@@ -2801,12 +2801,12 @@
       <c r="A70" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="22"/>
-      <c r="E70" s="22"/>
-      <c r="F70" s="22"/>
-      <c r="G70" s="23"/>
+      <c r="B70" s="27"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="27"/>
+      <c r="E70" s="27"/>
+      <c r="F70" s="27"/>
+      <c r="G70" s="28"/>
       <c r="H70" s="18">
         <v>45036</v>
       </c>
@@ -2825,12 +2825,12 @@
       <c r="A71" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="22"/>
-      <c r="C71" s="22"/>
-      <c r="D71" s="22"/>
-      <c r="E71" s="22"/>
-      <c r="F71" s="22"/>
-      <c r="G71" s="23"/>
+      <c r="B71" s="27"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="27"/>
+      <c r="E71" s="27"/>
+      <c r="F71" s="27"/>
+      <c r="G71" s="28"/>
       <c r="H71" s="18">
         <v>45035</v>
       </c>
@@ -2849,20 +2849,24 @@
       <c r="A72" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="B72" s="22"/>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="22"/>
-      <c r="F72" s="22"/>
-      <c r="G72" s="23"/>
+      <c r="B72" s="27"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="27"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="28"/>
       <c r="H72" s="18">
         <v>45038</v>
       </c>
       <c r="I72" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J72" s="19"/>
-      <c r="K72" s="19"/>
+      <c r="J72" s="19">
+        <v>1</v>
+      </c>
+      <c r="K72" s="18">
+        <v>45038</v>
+      </c>
       <c r="L72" s="4"/>
     </row>
     <row r="73" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
@@ -15294,6 +15298,40 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="A72:G72"/>
+    <mergeCell ref="A67:G67"/>
+    <mergeCell ref="A68:G68"/>
+    <mergeCell ref="A69:G69"/>
+    <mergeCell ref="A70:G70"/>
+    <mergeCell ref="A71:G71"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="A44:G44"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A47:G47"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A53:G53"/>
     <mergeCell ref="A59:G59"/>
     <mergeCell ref="A60:G60"/>
     <mergeCell ref="A65:G65"/>
@@ -15306,40 +15344,6 @@
     <mergeCell ref="A62:G62"/>
     <mergeCell ref="A63:G63"/>
     <mergeCell ref="A64:G64"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="A49:G49"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="A53:G53"/>
-    <mergeCell ref="A44:G44"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A47:G47"/>
-    <mergeCell ref="A48:G48"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A41:G41"/>
-    <mergeCell ref="A42:G42"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A72:G72"/>
-    <mergeCell ref="A67:G67"/>
-    <mergeCell ref="A68:G68"/>
-    <mergeCell ref="A69:G69"/>
-    <mergeCell ref="A70:G70"/>
-    <mergeCell ref="A71:G71"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15348,6 +15352,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010087EE1EC09A597E4C8C3B99C8872D8AE3" ma:contentTypeVersion="0" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="00d4df624c444888d37780811be33f83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8d2d35cd79d80d3b38601b74d693a05d">
     <xsd:element name="properties">
@@ -15461,33 +15480,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40B05868-E3C8-4C35-A51C-41D5A3BADEBB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78609003-DBD1-489F-A00D-E4A98DB536C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15502,9 +15498,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78609003-DBD1-489F-A00D-E4A98DB536C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40B05868-E3C8-4C35-A51C-41D5A3BADEBB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>